<commit_message>
Berechnungen, Tabellen und Kommentierungen
</commit_message>
<xml_diff>
--- a/Manuelle Kalibrierung.xlsx
+++ b/Manuelle Kalibrierung.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studium\AnalytikV2.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD0F73-509E-4F7F-8B3E-724D970120F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FC0D88-E2C9-4EF6-82F2-16C7B148A6AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="2805" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{DFE8C85E-67A7-48FD-AA0A-31EF262ACFEF}"/>
+    <workbookView xWindow="-4275" yWindow="4815" windowWidth="15375" windowHeight="7875" firstSheet="3" activeTab="3" xr2:uid="{DFE8C85E-67A7-48FD-AA0A-31EF262ACFEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten 1" sheetId="2" r:id="rId1"/>
     <sheet name="Daten 2" sheetId="1" r:id="rId2"/>
     <sheet name="Konzentration des Blei Messgerä" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Volumen</t>
   </si>
@@ -82,14 +83,23 @@
   <si>
     <t>Schnittpunkt</t>
   </si>
+  <si>
+    <t>Masse 1 mg</t>
+  </si>
+  <si>
+    <t>Masse 2 mg</t>
+  </si>
+  <si>
+    <t>Masse 3 in mg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -207,8 +217,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2621,7 +2631,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,8 +2756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B396974-5670-4F22-B6B1-EBE45B872994}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,7 +2983,10 @@
         <f t="shared" si="0"/>
         <v>0.97286103951880942</v>
       </c>
-      <c r="G18">
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" s="5">
         <f>H16/G16</f>
         <v>6.6064064414493266</v>
       </c>
@@ -2993,6 +3006,13 @@
         <f>ABS(B19-AVERAGE($B$19:$B$22))/_xlfn.STDEV.P($B$19:$B$22)</f>
         <v>1.2182296272903219</v>
       </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <f>AVERAGE(5.757,7.186)</f>
+        <v>6.4714999999999998</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -3005,6 +3025,13 @@
         <f t="shared" ref="E20:E22" si="1">ABS(B20-AVERAGE($B$19:$B$22))/_xlfn.STDEV.P($B$19:$B$22)</f>
         <v>0.74967977064019964</v>
       </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5">
+        <f>AVERAGE(5.906,7.487)</f>
+        <v>6.6965000000000003</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
@@ -3058,7 +3085,7 @@
         <v>-424</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E26" si="2">ABS(B24-AVERAGE($B$23:$B$26))/_xlfn.STDEV.P($B$23:$B$26)</f>
+        <f t="shared" ref="E24" si="2">ABS(B24-AVERAGE($B$23:$B$26))/_xlfn.STDEV.P($B$23:$B$26)</f>
         <v>0.57134416156356704</v>
       </c>
     </row>
@@ -3097,4 +3124,114 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350D7821-F525-4C18-B9F2-68962BA4928E}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>4*'Konzentration des Blei Messgerä'!G19*25*10^-3</f>
+        <v>0.64715</v>
+      </c>
+      <c r="B2">
+        <f>4*'Konzentration des Blei Messgerä'!G20*25*10^-3</f>
+        <v>0.66965000000000008</v>
+      </c>
+      <c r="C2">
+        <f>4*'Konzentration des Blei Messgerä'!G18*25*10^-3</f>
+        <v>0.66064064414493273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2*1000</f>
+        <v>647.15</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:C3" si="0">B2*1000</f>
+        <v>669.65000000000009</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>660.64064414493271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>AVERAGE('Konzentration des Blei Messgerä'!G18:G20)</f>
+        <v>6.5914688138164417</v>
+      </c>
+      <c r="C6">
+        <f>_xlfn.STDEV.P('Konzentration des Blei Messgerä'!G18:G20)</f>
+        <v>9.2461161357887969E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>(4.303/SQRT(3))*C6</f>
+        <v>0.22970479594731549</v>
+      </c>
+      <c r="C8">
+        <f>25*10^-3</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <f>C8*4*B8</f>
+        <v>2.2970479594731551E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>B13*1000</f>
+        <v>659.14688138164422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>C8*(B6+B8)*4</f>
+        <v>0.68211736097637576</v>
+      </c>
+      <c r="E11">
+        <f>D8*1000</f>
+        <v>22.97047959473155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>C8*(B6-B8)*4</f>
+        <v>0.6361764017869127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>C8*(B6-B9)*4</f>
+        <v>0.65914688138164423</v>
+      </c>
+      <c r="C13">
+        <f>B13+D8</f>
+        <v>0.68211736097637576</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>